<commit_message>
fix check permission bug
</commit_message>
<xml_diff>
--- a/backend/data/CSE Active HDR candidates staff details 210624.xlsx
+++ b/backend/data/CSE Active HDR candidates staff details 210624.xlsx
@@ -11,14 +11,14 @@
     <sheet name="CSE staff" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'HDR students'!$A$1:$H$232</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'HDR students'!$A$1:$H$233</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315">
   <si>
     <t>No</t>
   </si>
@@ -575,6 +575,78 @@
     <t>a</t>
   </si>
   <si>
+    <t>z2</t>
+  </si>
+  <si>
+    <t>z3</t>
+  </si>
+  <si>
+    <t>z4</t>
+  </si>
+  <si>
+    <t>z5</t>
+  </si>
+  <si>
+    <t>z6</t>
+  </si>
+  <si>
+    <t>z7</t>
+  </si>
+  <si>
+    <t>z8</t>
+  </si>
+  <si>
+    <t>z9</t>
+  </si>
+  <si>
+    <t>z10</t>
+  </si>
+  <si>
+    <t>z11</t>
+  </si>
+  <si>
+    <t>z12</t>
+  </si>
+  <si>
+    <t>z13</t>
+  </si>
+  <si>
+    <t>z14</t>
+  </si>
+  <si>
+    <t>z15</t>
+  </si>
+  <si>
+    <t>z16</t>
+  </si>
+  <si>
+    <t>z17</t>
+  </si>
+  <si>
+    <t>z18</t>
+  </si>
+  <si>
+    <t>z19</t>
+  </si>
+  <si>
+    <t>z20</t>
+  </si>
+  <si>
+    <t>z21</t>
+  </si>
+  <si>
+    <t>z22</t>
+  </si>
+  <si>
+    <t>z23</t>
+  </si>
+  <si>
+    <t>z24</t>
+  </si>
+  <si>
+    <t>z25</t>
+  </si>
+  <si>
     <t>Staff z ID</t>
   </si>
   <si>
@@ -876,9 +948,6 @@
   </si>
   <si>
     <t>Mech</t>
-  </si>
-  <si>
-    <t>z2</t>
   </si>
   <si>
     <t>Iding</t>
@@ -901,12 +970,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
@@ -914,11 +983,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
@@ -937,7 +1001,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,15 +1036,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -973,9 +1052,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -984,6 +1063,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -998,7 +1085,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -1014,14 +1101,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1035,20 +1122,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1057,17 +1130,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1081,13 +1145,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1102,13 +1166,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1126,19 +1214,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,7 +1226,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,19 +1238,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,13 +1262,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,13 +1286,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,61 +1334,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1325,6 +1383,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -1336,6 +1403,36 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1372,30 +1469,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1404,166 +1477,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1572,14 +1630,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -1921,10 +1979,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J233"/>
+  <dimension ref="A1:J257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="C235" sqref="I234 C235"/>
+    <sheetView tabSelected="1" topLeftCell="E231" workbookViewId="0">
+      <selection activeCell="J246" sqref="J246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83088235294118" defaultRowHeight="16.8"/>
@@ -9231,8 +9289,704 @@
         <v>184</v>
       </c>
     </row>
+    <row r="234" spans="1:10">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>185</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E234" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G234" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H234" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>186</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+      <c r="D235" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E235" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G235" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H235" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>187</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+      <c r="D236" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E236" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G236" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H236" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>188</v>
+      </c>
+      <c r="C237">
+        <v>4</v>
+      </c>
+      <c r="D237" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E237" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H237" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>189</v>
+      </c>
+      <c r="C238">
+        <v>5</v>
+      </c>
+      <c r="D238" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G238" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H238" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>190</v>
+      </c>
+      <c r="C239">
+        <v>6</v>
+      </c>
+      <c r="D239" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E239" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H239" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>191</v>
+      </c>
+      <c r="C240">
+        <v>7</v>
+      </c>
+      <c r="D240" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E240" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G240" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H240" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>192</v>
+      </c>
+      <c r="C241">
+        <v>8</v>
+      </c>
+      <c r="D241" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E241" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H241" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>193</v>
+      </c>
+      <c r="C242">
+        <v>9</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H242" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>194</v>
+      </c>
+      <c r="C243">
+        <v>10</v>
+      </c>
+      <c r="D243" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E243" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H243" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>195</v>
+      </c>
+      <c r="C244">
+        <v>11</v>
+      </c>
+      <c r="D244" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E244" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H244" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>196</v>
+      </c>
+      <c r="C245">
+        <v>12</v>
+      </c>
+      <c r="D245" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E245" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H245" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>197</v>
+      </c>
+      <c r="C246">
+        <v>13</v>
+      </c>
+      <c r="D246" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E246" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G246" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H246" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>198</v>
+      </c>
+      <c r="C247">
+        <v>14</v>
+      </c>
+      <c r="D247" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E247" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H247" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>199</v>
+      </c>
+      <c r="C248">
+        <v>15</v>
+      </c>
+      <c r="D248" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E248" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G248" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H248" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>200</v>
+      </c>
+      <c r="C249">
+        <v>16</v>
+      </c>
+      <c r="D249" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E249" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F249" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H249" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>201</v>
+      </c>
+      <c r="C250">
+        <v>17</v>
+      </c>
+      <c r="D250" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E250" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F250" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G250" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H250" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>202</v>
+      </c>
+      <c r="C251">
+        <v>18</v>
+      </c>
+      <c r="D251" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E251" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G251" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H251" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>203</v>
+      </c>
+      <c r="C252">
+        <v>19</v>
+      </c>
+      <c r="D252" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E252" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H252" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>204</v>
+      </c>
+      <c r="C253">
+        <v>20</v>
+      </c>
+      <c r="D253" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E253" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F253" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H253" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>205</v>
+      </c>
+      <c r="C254">
+        <v>21</v>
+      </c>
+      <c r="D254" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E254" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F254" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G254" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H254" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>206</v>
+      </c>
+      <c r="C255">
+        <v>22</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E255" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F255" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G255" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H255" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>207</v>
+      </c>
+      <c r="C256">
+        <v>23</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E256" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F256" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G256" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H256" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>208</v>
+      </c>
+      <c r="C257">
+        <v>24</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E257" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="F257" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G257" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H257" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J257">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H232"/>
+  <autoFilter ref="A1:H233"/>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
@@ -9262,10 +10016,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -9280,10 +10034,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
@@ -9294,29 +10048,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E2" s="3" t="str">
         <f>C2&amp;"@"&amp;D2</f>
         <v>aooif@unsw.edu.au</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>51</v>
@@ -9327,29 +10081,29 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E61" si="0">C3&amp;"@"&amp;D3</f>
         <v>hyhsy@unsw.edu.au</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>52</v>
@@ -9360,29 +10114,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tjfxr@unsw.edu.au</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>53</v>
@@ -9393,29 +10147,29 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>tzoyy@unsw.edu.au</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>54</v>
@@ -9426,29 +10180,29 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>kjkkx@unsw.edu.au</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>55</v>
@@ -9459,29 +10213,29 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>trgje@unsw.edu.au</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>56</v>
@@ -9492,29 +10246,29 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mzzpu@unsw.edu.au</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>57</v>
@@ -9525,29 +10279,29 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ytsce@unsw.edu.au</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>58</v>
@@ -9558,29 +10312,29 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>jluty@unsw.edu.au</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>59</v>
@@ -9591,29 +10345,29 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>jfvyy@unsw.edu.au</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="J11" s="6">
         <v>12344</v>
@@ -9624,29 +10378,29 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>xjqxo@unsw.edu.au</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>61</v>
@@ -9657,29 +10411,29 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>vkmlm@unsw.edu.au</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>63</v>
@@ -9690,29 +10444,29 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>jgxuq@unsw.edu.au</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>64</v>
@@ -9723,29 +10477,29 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dbpvo@unsw.edu.au</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>65</v>
@@ -9756,29 +10510,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ogari@unsw.edu.au</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>66</v>
@@ -9789,29 +10543,29 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>croav@unsw.edu.au</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>67</v>
@@ -9822,29 +10576,29 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>xjmmj@unsw.edu.au</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>68</v>
@@ -9855,29 +10609,29 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>abvgn@unsw.edu.au</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J19" s="6" t="s">
         <v>69</v>
@@ -9888,29 +10642,29 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>lpgyy@unsw.edu.au</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>71</v>
@@ -9921,29 +10675,29 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ygjby@unsw.edu.au</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>73</v>
@@ -9954,29 +10708,29 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>xqaqw@unsw.edu.au</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>74</v>
@@ -9987,29 +10741,29 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>lkiki@unsw.edu.au</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>75</v>
@@ -10020,29 +10774,29 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>psml@unsw.edu.au</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>77</v>
@@ -10053,29 +10807,29 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>zesqr@unsw.edu.au</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>79</v>
@@ -10086,29 +10840,29 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>qwjgy@unsw.edu.au</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>80</v>
@@ -10119,29 +10873,29 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>bvljb@unsw.edu.au</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>81</v>
@@ -10152,29 +10906,29 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>rjpju@unsw.edu.au</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>82</v>
@@ -10185,29 +10939,29 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>liqqz@unsw.edu.au</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>83</v>
@@ -10218,29 +10972,29 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gmfzg@unsw.edu.au</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>84</v>
@@ -10251,29 +11005,29 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>achdi@unsw.edu.au</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>85</v>
@@ -10284,29 +11038,29 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>aowom@unsw.edu.au</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>86</v>
@@ -10317,29 +11071,29 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>vsxla@unsw.edu.au</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J33" s="7" t="s">
         <v>87</v>
@@ -10350,29 +11104,29 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>pczae@unsw.edu.au</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>88</v>
@@ -10383,29 +11137,29 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>zgwrl@unsw.edu.au</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J35" s="7" t="s">
         <v>89</v>
@@ -10416,29 +11170,29 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>uwnoi@unsw.edu.au</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>90</v>
@@ -10449,29 +11203,29 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ofjzr@unsw.edu.au</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>92</v>
@@ -10482,29 +11236,29 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dcrkv@unsw.edu.au</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>94</v>
@@ -10515,29 +11269,29 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>jnsrf@unsw.edu.au</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>95</v>
@@ -10548,29 +11302,29 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mqrci@unsw.edu.au</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J40" s="7" t="s">
         <v>97</v>
@@ -10581,29 +11335,29 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>whjat@unsw.edu.au</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J41" s="7" t="s">
         <v>99</v>
@@ -10614,29 +11368,29 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>oshgy@unsw.edu.au</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>100</v>
@@ -10647,29 +11401,29 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ggeqk@unsw.edu.au</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J43" s="7" t="s">
         <v>101</v>
@@ -10680,29 +11434,29 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ncxdi@unsw.edu.au</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>102</v>
@@ -10713,29 +11467,29 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>fjujf@unsw.edu.au</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J45" s="7" t="s">
         <v>103</v>
@@ -10746,29 +11500,29 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dfddd@unsw.edu.au</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J46" s="7" t="s">
         <v>104</v>
@@ -10779,29 +11533,29 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>gftyu@unsw.edu.au</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J47" s="7" t="s">
         <v>105</v>
@@ -10812,29 +11566,29 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dsf ss@unsw.edu.au</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J48" s="7" t="s">
         <v>106</v>
@@ -10845,29 +11599,29 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dsfsfs@unsw.edu.au</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J49" s="7" t="s">
         <v>108</v>
@@ -10878,29 +11632,29 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>eydzs s@unsw.edu.au</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J50" s="7" t="s">
         <v>110</v>
@@ -10911,29 +11665,29 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>dtyd @unsw.edu.au</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J51" s="7" t="s">
         <v>111</v>
@@ -10944,29 +11698,29 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>fgfd ss@unsw.edu.au</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>84</v>
@@ -10977,29 +11731,29 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>fdy rea@unsw.edu.au</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>85</v>
@@ -11010,29 +11764,29 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>kiuns@unsw.edu.au</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>86</v>
@@ -11043,29 +11797,29 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>mxivj @unsw.edu.au</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J55" s="7" t="s">
         <v>87</v>
@@ -11076,29 +11830,29 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>m  hs@unsw.edu.au</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J56" s="7" t="s">
         <v>88</v>
@@ -11109,29 +11863,29 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>s ffdg@unsw.edu.au</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J57" s="7" t="s">
         <v>89</v>
@@ -11142,29 +11896,29 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>fgfffs@unsw.edu.au</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J58" s="7" t="s">
         <v>90</v>
@@ -11175,29 +11929,29 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>d dg dh@unsw.edu.au</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J59" s="7" t="s">
         <v>92</v>
@@ -11208,29 +11962,29 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>fdgds@unsw.edu.au</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J60" s="7" t="s">
         <v>94</v>
@@ -11241,29 +11995,29 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>ddbgf yb@unsw.edu.au</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="J61" s="7" t="s">
         <v>95</v>
@@ -11274,31 +12028,31 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>286</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E62" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G62" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J62" s="7" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -11306,28 +12060,28 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="C63" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E63" t="s">
         <v>180</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="G63" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="J63" s="7">
         <v>12345678</v>

</xml_diff>

<commit_message>
fix express book bug
</commit_message>
<xml_diff>
--- a/backend/data/CSE Active HDR candidates staff details 210624.xlsx
+++ b/backend/data/CSE Active HDR candidates staff details 210624.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310">
   <si>
     <t>No</t>
   </si>
@@ -939,6 +939,15 @@
   </si>
   <si>
     <t>Administrator</t>
+  </si>
+  <si>
+    <t>z7</t>
+  </si>
+  <si>
+    <t>non_cse</t>
+  </si>
+  <si>
+    <t>7@qq.com</t>
   </si>
 </sst>
 </file>
@@ -947,9 +956,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -992,10 +1001,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1014,15 +1024,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1043,7 +1045,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -1055,6 +1057,14 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1074,31 +1084,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1112,6 +1106,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1120,8 +1128,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1142,25 +1151,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1172,13 +1175,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,13 +1211,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,109 +1325,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1353,6 +1362,15 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1404,17 +1422,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1447,103 +1454,105 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1552,28 +1561,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1582,22 +1591,22 @@
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1612,11 +1621,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="41" applyFill="1" applyAlignment="1"/>
   </cellXfs>
@@ -2006,7 +2015,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4039,7 +4048,7 @@
         <v>14</v>
       </c>
       <c r="I66" s="3"/>
-      <c r="J66" s="9" t="s">
+      <c r="J66" s="10" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7762,7 +7771,7 @@
         <v>14</v>
       </c>
       <c r="I185" s="3"/>
-      <c r="J185" s="9" t="s">
+      <c r="J185" s="10" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9211,19 +9220,19 @@
       </c>
     </row>
     <row r="232" spans="1:10">
-      <c r="A232" s="10">
+      <c r="A232" s="11">
         <v>231</v>
       </c>
-      <c r="B232" s="10" t="s">
+      <c r="B232" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C232" s="10" t="s">
+      <c r="C232" s="11" t="s">
         <v>179</v>
       </c>
       <c r="D232" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E232" s="11" t="s">
+      <c r="E232" s="12" t="s">
         <v>180</v>
       </c>
       <c r="F232" s="3" t="s">
@@ -9252,7 +9261,7 @@
       <c r="D233" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E233" s="12" t="s">
+      <c r="E233" s="8" t="s">
         <v>183</v>
       </c>
       <c r="F233" s="3" t="s">
@@ -9386,140 +9395,140 @@
     </row>
     <row r="238" spans="4:8">
       <c r="D238" s="4"/>
-      <c r="E238" s="11"/>
+      <c r="E238" s="12"/>
       <c r="F238" s="3"/>
       <c r="G238" s="3"/>
       <c r="H238" s="3"/>
     </row>
     <row r="239" spans="4:8">
       <c r="D239" s="4"/>
-      <c r="E239" s="11"/>
+      <c r="E239" s="12"/>
       <c r="F239" s="3"/>
       <c r="G239" s="3"/>
       <c r="H239" s="3"/>
     </row>
     <row r="240" spans="4:8">
       <c r="D240" s="4"/>
-      <c r="E240" s="11"/>
+      <c r="E240" s="12"/>
       <c r="F240" s="3"/>
       <c r="G240" s="3"/>
       <c r="H240" s="3"/>
     </row>
     <row r="241" spans="4:8">
       <c r="D241" s="4"/>
-      <c r="E241" s="11"/>
+      <c r="E241" s="12"/>
       <c r="F241" s="3"/>
       <c r="G241" s="3"/>
       <c r="H241" s="3"/>
     </row>
     <row r="242" spans="4:8">
       <c r="D242" s="4"/>
-      <c r="E242" s="11"/>
+      <c r="E242" s="12"/>
       <c r="F242" s="3"/>
       <c r="G242" s="3"/>
       <c r="H242" s="3"/>
     </row>
     <row r="243" spans="4:8">
       <c r="D243" s="4"/>
-      <c r="E243" s="11"/>
+      <c r="E243" s="12"/>
       <c r="F243" s="3"/>
       <c r="G243" s="3"/>
       <c r="H243" s="3"/>
     </row>
     <row r="244" spans="4:8">
       <c r="D244" s="4"/>
-      <c r="E244" s="11"/>
+      <c r="E244" s="12"/>
       <c r="F244" s="3"/>
       <c r="G244" s="3"/>
       <c r="H244" s="3"/>
     </row>
     <row r="245" spans="4:8">
       <c r="D245" s="4"/>
-      <c r="E245" s="11"/>
+      <c r="E245" s="12"/>
       <c r="F245" s="3"/>
       <c r="G245" s="3"/>
       <c r="H245" s="3"/>
     </row>
     <row r="246" spans="4:8">
       <c r="D246" s="4"/>
-      <c r="E246" s="11"/>
+      <c r="E246" s="12"/>
       <c r="F246" s="3"/>
       <c r="G246" s="3"/>
       <c r="H246" s="3"/>
     </row>
     <row r="247" spans="4:8">
       <c r="D247" s="4"/>
-      <c r="E247" s="11"/>
+      <c r="E247" s="12"/>
       <c r="F247" s="3"/>
       <c r="G247" s="3"/>
       <c r="H247" s="3"/>
     </row>
     <row r="248" spans="4:8">
       <c r="D248" s="4"/>
-      <c r="E248" s="11"/>
+      <c r="E248" s="12"/>
       <c r="F248" s="3"/>
       <c r="G248" s="3"/>
       <c r="H248" s="3"/>
     </row>
     <row r="249" spans="4:8">
       <c r="D249" s="4"/>
-      <c r="E249" s="11"/>
+      <c r="E249" s="12"/>
       <c r="F249" s="3"/>
       <c r="G249" s="3"/>
       <c r="H249" s="3"/>
     </row>
     <row r="250" spans="4:8">
       <c r="D250" s="4"/>
-      <c r="E250" s="11"/>
+      <c r="E250" s="12"/>
       <c r="F250" s="3"/>
       <c r="G250" s="3"/>
       <c r="H250" s="3"/>
     </row>
     <row r="251" spans="4:8">
       <c r="D251" s="4"/>
-      <c r="E251" s="11"/>
+      <c r="E251" s="12"/>
       <c r="F251" s="3"/>
       <c r="G251" s="3"/>
       <c r="H251" s="3"/>
     </row>
     <row r="252" spans="4:8">
       <c r="D252" s="4"/>
-      <c r="E252" s="11"/>
+      <c r="E252" s="12"/>
       <c r="F252" s="3"/>
       <c r="G252" s="3"/>
       <c r="H252" s="3"/>
     </row>
     <row r="253" spans="4:8">
       <c r="D253" s="4"/>
-      <c r="E253" s="11"/>
+      <c r="E253" s="12"/>
       <c r="F253" s="3"/>
       <c r="G253" s="3"/>
       <c r="H253" s="3"/>
     </row>
     <row r="254" spans="4:8">
       <c r="D254" s="4"/>
-      <c r="E254" s="11"/>
+      <c r="E254" s="12"/>
       <c r="F254" s="3"/>
       <c r="G254" s="3"/>
       <c r="H254" s="3"/>
     </row>
     <row r="255" spans="4:8">
       <c r="D255" s="4"/>
-      <c r="E255" s="11"/>
+      <c r="E255" s="12"/>
       <c r="F255" s="3"/>
       <c r="G255" s="3"/>
       <c r="H255" s="3"/>
     </row>
     <row r="256" spans="4:8">
       <c r="D256" s="4"/>
-      <c r="E256" s="11"/>
+      <c r="E256" s="12"/>
       <c r="F256" s="3"/>
       <c r="G256" s="3"/>
       <c r="H256" s="3"/>
     </row>
     <row r="257" spans="4:8">
       <c r="D257" s="4"/>
-      <c r="E257" s="11"/>
+      <c r="E257" s="12"/>
       <c r="F257" s="3"/>
       <c r="G257" s="3"/>
       <c r="H257" s="3"/>
@@ -9542,10 +9551,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83088235294118" defaultRowHeight="16.8"/>
@@ -11665,7 +11674,42 @@
         <v>1</v>
       </c>
     </row>
+    <row r="65" spans="1:10">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>307</v>
+      </c>
+      <c r="C65" t="s">
+        <v>308</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" t="s">
+        <v>297</v>
+      </c>
+      <c r="H65" t="s">
+        <v>210</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="J65" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E65" r:id="rId1" display="7@qq.com" tooltip="mailto:7@qq.com"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>